<commit_message>
add novas funções de teste para numeros negativos, strings em listas e apenas uma string
</commit_message>
<xml_diff>
--- a/exxemplo de test.xlsx
+++ b/exxemplo de test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\escola-teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{163F626B-1B92-4775-BB68-584824F87890}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E14D7C7-DA05-4791-BEC3-C1BE9041F0AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{4540C33A-8685-4F46-8320-4A5D2AE8E085}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>notas</t>
   </si>
@@ -126,9 +126,6 @@
     <t>ValueError("lista invalida, lista vazia")</t>
   </si>
   <si>
-    <t>ValueError("lista invalida, não suportado (String)")</t>
-  </si>
-  <si>
     <t>[ ]</t>
   </si>
   <si>
@@ -142,6 +139,18 @@
   </si>
   <si>
     <t>ValueError("valor não esta entre 0 e 10")</t>
+  </si>
+  <si>
+    <t>TypeError("lista invalida, não suportado (String)")</t>
+  </si>
+  <si>
+    <t>"ola"</t>
+  </si>
+  <si>
+    <t>enviando uma string</t>
+  </si>
+  <si>
+    <t>TypeError("não é uma lista")</t>
   </si>
 </sst>
 </file>
@@ -538,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{466E04FD-D52F-45E6-BDC4-3836C645B30D}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,10 +773,10 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>32</v>
@@ -781,13 +790,13 @@
         <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -804,7 +813,24 @@
         <v>22</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>